<commit_message>
cadastro de grupo de funcionario e criando venda + documentoação
</commit_message>
<xml_diff>
--- a/documentacao/planilha de status e pendencias.xlsx
+++ b/documentacao/planilha de status e pendencias.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\facul 2019 -1 semestre\pratica\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\facul 2019 -1 semestre\projeto_pratica_profissional\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F249EB20-61D4-4689-A798-CF3AD830F55D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B46449C-E3C2-4923-9B53-09C032CE46EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FAD85956-36FA-4642-B593-81A4321B0BA2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t>tarefas</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>cad cond pag tbm n vem selecionado após o cad no pesquisar</t>
+  </si>
+  <si>
+    <t>adicionar id do fornecedor como primary key na ccompra, assim como no desbloqueio da tela de nova</t>
   </si>
 </sst>
 </file>
@@ -487,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C4F633-CFB7-4344-8A5E-EE0334BEE044}">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +585,7 @@
         <v>25</v>
       </c>
       <c r="R6" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -695,8 +698,16 @@
         <v>26</v>
       </c>
     </row>
+    <row r="17" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>37</v>
+      </c>
+      <c r="R17" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="O5:O1048576 R1:R4 R6:R11 R13 R15:R16">
+  <conditionalFormatting sqref="O5:O1048576 R1:R4 R6:R11 R13 R15:R17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="formula" val="&quot;OK=$Pendente$&quot;"/>

</xml_diff>